<commit_message>
Predicate abstraction added chap 2
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="7635" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Fischer" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <definedName name="benchmark_token_3" localSheetId="3">Munka1!$A$168:$E$227</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -110,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2125" uniqueCount="29">
   <si>
     <t>Fischer</t>
   </si>
@@ -194,6 +193,9 @@
   </si>
   <si>
     <t>SUT</t>
+  </si>
+  <si>
+    <t>SP</t>
   </si>
 </sst>
 </file>
@@ -581,7 +583,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Fischer!$N$7</c:f>
+              <c:f>Fischer!$N$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -625,7 +627,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Fischer!$O$7:$S$7</c:f>
+              <c:f>Fischer!$O$8:$S$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -649,7 +651,6 @@
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -659,11 +660,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1065265008"/>
-        <c:axId val="-1065263920"/>
+        <c:axId val="1712392256"/>
+        <c:axId val="1712386816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1065265008"/>
+        <c:axId val="1712392256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -762,7 +763,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1065263920"/>
+        <c:crossAx val="1712386816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -770,7 +771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1065263920"/>
+        <c:axId val="1712386816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40000"/>
@@ -879,7 +880,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1065265008"/>
+        <c:crossAx val="1712392256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -960,7 +961,1041 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="hu-HU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.3060804259167123E-2"/>
+          <c:y val="6.9386200966257708E-2"/>
+          <c:w val="0.82559058068303159"/>
+          <c:h val="0.74167658037743944"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka1!$I$43:$I$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka1!$K$43:$K$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-0.24412514432750862</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.2757241303992109</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3078443483419682E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59328606702045716</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.62428209583566818</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2387985627139169</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6232492903979003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3516610517906722</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1030267677443413</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.3451907589501193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka1!$I$43:$I$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka1!$K$43:$K$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-0.24412514432750862</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.2757241303992109</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3078443483419682E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59328606702045716</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.62428209583566818</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2387985627139169</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6232492903979003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3516610517906722</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1030267677443413</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.3451907589501193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1683930848"/>
+        <c:axId val="1683928672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1683930848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="50"/>
+          <c:min val="5"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="1683928672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1683928672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1683930848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr rot="0"/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="hu-HU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fischer!$N$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>STU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fischer!$O$2:$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CSMA2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSMA3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSMA4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fisch2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fisch3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fischer!$O$3:$S$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1049</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9753.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fischer!$N$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SGU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fischer!$O$2:$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CSMA2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSMA3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSMA4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fisch2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fisch3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fischer!$O$4:$S$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>446.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>703.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1377</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35183</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fischer!$N$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>STT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fischer!$O$2:$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CSMA2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSMA3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSMA4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fisch2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fisch3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fischer!$O$5:$S$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1113.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9808</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fischer!$N$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SGT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fischer!$O$2:$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CSMA2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSMA3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSMA4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fisch2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fisch3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fischer!$O$6:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>317</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9883</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>426.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6783.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fischer!$N$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fischer!$O$2:$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CSMA2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSMA3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSMA4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fisch2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fisch3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fischer!$O$7:$S$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3151</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30845</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2224</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Fischer!$N$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AZ</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fischer!$O$2:$S$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CSMA2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CSMA3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CSMA4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fisch2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fisch3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fischer!$O$8:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>557</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2098</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27826</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>888</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9294</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1959285072"/>
+        <c:axId val="1959286160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1959285072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1959286160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1959286160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="39999"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1959285072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -1102,11 +2137,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1065268272"/>
-        <c:axId val="-1065273168"/>
+        <c:axId val="1712387360"/>
+        <c:axId val="1712397152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1065268272"/>
+        <c:axId val="1712387360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +2184,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1065273168"/>
+        <c:crossAx val="1712397152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1157,7 +2192,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1065273168"/>
+        <c:axId val="1712397152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1208,7 +2243,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1065268272"/>
+        <c:crossAx val="1712387360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1257,7 +2292,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -1399,11 +2434,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1065273712"/>
-        <c:axId val="-1065275344"/>
+        <c:axId val="1712388448"/>
+        <c:axId val="1712390080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1065273712"/>
+        <c:axId val="1712388448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1446,7 +2481,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1065275344"/>
+        <c:crossAx val="1712390080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1454,7 +2489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1065275344"/>
+        <c:axId val="1712390080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1505,7 +2540,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1065273712"/>
+        <c:crossAx val="1712388448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1554,7 +2589,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -1701,11 +2736,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1065261200"/>
-        <c:axId val="-1065262288"/>
+        <c:axId val="1712398240"/>
+        <c:axId val="1712391712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1065261200"/>
+        <c:axId val="1712398240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1748,7 +2783,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1065262288"/>
+        <c:crossAx val="1712391712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1756,7 +2791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1065262288"/>
+        <c:axId val="1712391712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1807,7 +2842,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1065261200"/>
+        <c:crossAx val="1712398240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1856,7 +2891,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -2665,11 +3700,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1065274256"/>
-        <c:axId val="-1065267184"/>
+        <c:axId val="1668886048"/>
+        <c:axId val="1683930304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1065274256"/>
+        <c:axId val="1668886048"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -2784,12 +3819,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1065267184"/>
+        <c:crossAx val="1683930304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1065267184"/>
+        <c:axId val="1683930304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2902,7 +3937,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1065274256"/>
+        <c:crossAx val="1668886048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2951,7 +3986,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -3202,11 +4237,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-883823408"/>
-        <c:axId val="-883829392"/>
+        <c:axId val="1683933024"/>
+        <c:axId val="1683931936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-883823408"/>
+        <c:axId val="1683933024"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3264,12 +4299,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-883829392"/>
+        <c:crossAx val="1683931936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-883829392"/>
+        <c:axId val="1683931936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3326,7 +4361,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-883823408"/>
+        <c:crossAx val="1683933024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3375,7 +4410,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -3468,11 +4503,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-975899360"/>
-        <c:axId val="-975908064"/>
+        <c:axId val="1683932480"/>
+        <c:axId val="1683927584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-975899360"/>
+        <c:axId val="1683932480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3504,7 +4539,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3571,7 +4605,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-975908064"/>
+        <c:crossAx val="1683927584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3579,7 +4613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-975908064"/>
+        <c:axId val="1683927584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3625,7 +4659,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3686,7 +4719,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-975899360"/>
+        <c:crossAx val="1683932480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3735,7 +4768,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
@@ -3866,11 +4899,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-975899904"/>
-        <c:axId val="-975897184"/>
+        <c:axId val="1683937376"/>
+        <c:axId val="1683938464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-975899904"/>
+        <c:axId val="1683937376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
@@ -3918,7 +4951,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3985,12 +5017,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-975897184"/>
+        <c:crossAx val="1683938464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-975897184"/>
+        <c:axId val="1683938464"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4038,7 +5070,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4105,7 +5136,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-975899904"/>
+        <c:crossAx val="1683937376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4154,374 +5185,47 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="2.3060804259167123E-2"/>
-          <c:y val="6.9386200966257708E-2"/>
-          <c:w val="0.82559058068303159"/>
-          <c:h val="0.74167658037743944"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Munka1!$I$43:$I$52</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Munka1!$K$43:$K$52</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>-0.24412514432750862</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-0.2757241303992109</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.3078443483419682E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.59328606702045716</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.62428209583566818</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.2387985627139169</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.6232492903979003</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.3516610517906722</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.1030267677443413</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.3451907589501193</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="12700" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Munka1!$I$43:$I$52</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Munka1!$K$43:$K$52</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>-0.24412514432750862</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-0.2757241303992109</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.3078443483419682E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.59328606702045716</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.62428209583566818</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.2387985627139169</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.6232492903979003</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.3516610517906722</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.1030267677443413</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.3451907589501193</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="t"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-878425920"/>
-        <c:axId val="-878435168"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="-878425920"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="50"/>
-          <c:min val="5"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="low"/>
-        <c:crossAx val="-878435168"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="-878435168"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-878425920"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:noFill/>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr rot="0"/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="hu-HU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5365,6 +6069,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6894,7 +8114,7 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6921,8 +8141,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -7023,7 +8243,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -7055,10 +8275,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -7098,23 +8318,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -7219,8 +8438,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -7352,20 +8571,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -7379,17 +8597,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -7926,509 +9133,6 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8925,6 +9629,509 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -9464,16 +10671,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9487,6 +10694,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagram 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10041,8 +11278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S114"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="Z30" sqref="Z30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10335,22 +11572,22 @@
         <v>5842.5</v>
       </c>
       <c r="N7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="O7">
-        <v>557</v>
+        <v>329</v>
       </c>
       <c r="P7">
-        <v>2098</v>
+        <v>3151</v>
       </c>
       <c r="Q7">
-        <v>27826</v>
+        <v>30845</v>
       </c>
       <c r="R7">
-        <v>888</v>
+        <v>90</v>
       </c>
       <c r="S7">
-        <v>9294</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -10380,6 +11617,24 @@
       </c>
       <c r="K8">
         <v>426.5</v>
+      </c>
+      <c r="N8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8">
+        <v>557</v>
+      </c>
+      <c r="P8">
+        <v>2098</v>
+      </c>
+      <c r="Q8">
+        <v>27826</v>
+      </c>
+      <c r="R8">
+        <v>888</v>
+      </c>
+      <c r="S8">
+        <v>9294</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -12768,7 +14023,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L2926"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2905" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2905" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Y2927" sqref="Y2927"/>
     </sheetView>
   </sheetViews>
@@ -33257,7 +34512,7 @@
         <v>2</v>
       </c>
       <c r="G2916">
-        <f>AVERAGE(G2904:J2904)</f>
+        <f t="shared" ref="G2916:G2926" si="0">AVERAGE(G2904:J2904)</f>
         <v>776.5</v>
       </c>
       <c r="H2916">
@@ -33269,7 +34524,7 @@
         <v>4</v>
       </c>
       <c r="G2917">
-        <f>AVERAGE(G2905:J2905)</f>
+        <f t="shared" si="0"/>
         <v>583.75</v>
       </c>
       <c r="H2917">
@@ -33281,7 +34536,7 @@
         <v>8</v>
       </c>
       <c r="G2918">
-        <f>AVERAGE(G2906:J2906)</f>
+        <f t="shared" si="0"/>
         <v>1126.25</v>
       </c>
       <c r="H2918">
@@ -33293,7 +34548,7 @@
         <v>16</v>
       </c>
       <c r="G2919">
-        <f>AVERAGE(G2907:J2907)</f>
+        <f t="shared" si="0"/>
         <v>1234.5</v>
       </c>
       <c r="H2919">
@@ -33305,7 +34560,7 @@
         <v>32</v>
       </c>
       <c r="G2920">
-        <f>AVERAGE(G2908:J2908)</f>
+        <f t="shared" si="0"/>
         <v>1621</v>
       </c>
     </row>
@@ -33314,7 +34569,7 @@
         <v>64</v>
       </c>
       <c r="G2921">
-        <f>AVERAGE(G2909:J2909)</f>
+        <f t="shared" si="0"/>
         <v>2700</v>
       </c>
     </row>
@@ -33323,7 +34578,7 @@
         <v>128</v>
       </c>
       <c r="G2922">
-        <f>AVERAGE(G2910:J2910)</f>
+        <f t="shared" si="0"/>
         <v>4893.25</v>
       </c>
     </row>
@@ -33332,7 +34587,7 @@
         <v>256</v>
       </c>
       <c r="G2923">
-        <f>AVERAGE(G2911:J2911)</f>
+        <f t="shared" si="0"/>
         <v>7955.5</v>
       </c>
     </row>
@@ -33341,7 +34596,7 @@
         <v>512</v>
       </c>
       <c r="G2924">
-        <f>AVERAGE(G2912:J2912)</f>
+        <f t="shared" si="0"/>
         <v>12285</v>
       </c>
     </row>
@@ -33350,7 +34605,7 @@
         <v>1024</v>
       </c>
       <c r="G2925">
-        <f>AVERAGE(G2913:J2913)</f>
+        <f t="shared" si="0"/>
         <v>43085.75</v>
       </c>
     </row>
@@ -33359,7 +34614,7 @@
         <v>2048</v>
       </c>
       <c r="G2926">
-        <f>AVERAGE(G2914:J2914)</f>
+        <f t="shared" si="0"/>
         <v>105343</v>
       </c>
     </row>
@@ -34202,7 +35457,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="K43">
-        <f>LOG(J32,10)</f>
+        <f t="shared" ref="K43:K52" si="0">LOG(J32,10)</f>
         <v>-0.24412514432750862</v>
       </c>
     </row>
@@ -34229,7 +35484,7 @@
         <v>0.53</v>
       </c>
       <c r="K44">
-        <f>LOG(J33,10)</f>
+        <f t="shared" si="0"/>
         <v>-0.2757241303992109</v>
       </c>
     </row>
@@ -34256,7 +35511,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="K45">
-        <f>LOG(J34,10)</f>
+        <f t="shared" si="0"/>
         <v>5.3078443483419682E-2</v>
       </c>
     </row>
@@ -34287,7 +35542,7 @@
         <v>3.92</v>
       </c>
       <c r="K46">
-        <f>LOG(J35,10)</f>
+        <f t="shared" si="0"/>
         <v>0.59328606702045716</v>
       </c>
     </row>
@@ -34314,7 +35569,7 @@
         <v>4.21</v>
       </c>
       <c r="K47">
-        <f>LOG(J36,10)</f>
+        <f t="shared" si="0"/>
         <v>0.62428209583566818</v>
       </c>
     </row>
@@ -34341,7 +35596,7 @@
         <v>17.329999999999998</v>
       </c>
       <c r="K48">
-        <f>LOG(J37,10)</f>
+        <f t="shared" si="0"/>
         <v>1.2387985627139169</v>
       </c>
     </row>
@@ -34368,7 +35623,7 @@
         <v>42</v>
       </c>
       <c r="K49">
-        <f>LOG(J38,10)</f>
+        <f t="shared" si="0"/>
         <v>1.6232492903979003</v>
       </c>
     </row>
@@ -34395,7 +35650,7 @@
         <v>224.73</v>
       </c>
       <c r="K50">
-        <f>LOG(J39,10)</f>
+        <f t="shared" si="0"/>
         <v>2.3516610517906722</v>
       </c>
     </row>
@@ -34422,7 +35677,7 @@
         <v>1267.73</v>
       </c>
       <c r="K51">
-        <f>LOG(J40,10)</f>
+        <f t="shared" si="0"/>
         <v>3.1030267677443413</v>
       </c>
     </row>
@@ -34452,7 +35707,7 @@
         <v>22140.67</v>
       </c>
       <c r="K52">
-        <f>LOG(J41,10)</f>
+        <f t="shared" si="0"/>
         <v>4.3451907589501193</v>
       </c>
     </row>

</xml_diff>